<commit_message>
13 Dev Changes commit
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LenskartTestData.xlsx
+++ b/src/test/resources/testdata/LenskartTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{97D07F8C-8588-432D-81F6-9CEB569F53AA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E9D65E24-30CF-4DA6-A64C-793B9DBBCC82}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15948" windowHeight="2928" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15948" windowHeight="4212" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserData" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="RepoIntegrationData" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0" refMode="R1C1"/>
-  <oleSize ref="A5:F8"/>
+  <oleSize ref="A6:G17"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="245">
   <si>
     <t>username</t>
   </si>
@@ -757,6 +757,12 @@
   <si>
     <t>test-juno-buildx</t>
   </si>
+  <si>
+    <t>ReplayPipeline</t>
+  </si>
+  <si>
+    <t>Preprod-pipeline</t>
+  </si>
 </sst>
 </file>
 
@@ -1405,8 +1411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33546052-E966-4F68-882D-901C990EE3E6}">
   <dimension ref="A1:XFD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35375,15 +35381,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7161A4-3871-41B8-AFD3-D2E01A42417C}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="48.77734375" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" customWidth="1"/>
     <col min="5" max="5" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.44140625" customWidth="1"/>
@@ -36212,7 +36218,31 @@
       </c>
       <c r="P17" s="8"/>
     </row>
-    <row r="18" spans="1:21" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="1:21" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27">
+        <v>1</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="P18" s="8"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>

</xml_diff>